<commit_message>
Agregación de requisitos y cambios de los casos de uso
</commit_message>
<xml_diff>
--- a/CRIALED/DOCUMENTOS/Matriz de trazabilidád.xlsx
+++ b/CRIALED/DOCUMENTOS/Matriz de trazabilidád.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aless\Documents\apli\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CRIALED\CRIALED---APLICACIONES-INFORM-TICAS-II\CRIALED\DOCUMENTOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF338CC3-44E9-4BDA-9D6C-56AB44B11BA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4DD07E7-A0A8-4675-A3B5-C1E44D2AC403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plantilla de matriz requisitos" sheetId="1" r:id="rId1"/>
@@ -612,7 +612,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -791,7 +791,7 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -803,7 +803,7 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1034,8 +1034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="64" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" zoomScale="64" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>